<commit_message>
Fix Indentation and Force Numero to Int64
</commit_message>
<xml_diff>
--- a/reconciliation.xlsx
+++ b/reconciliation.xlsx
@@ -481,10 +481,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>237650353920</t>
-        </is>
+      <c r="A2" t="n">
+        <v>237650353920</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -520,10 +518,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>237650874464</t>
-        </is>
+      <c r="A3" t="n">
+        <v>237650874464</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -559,10 +555,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>237650934256</t>
-        </is>
+      <c r="A4" t="n">
+        <v>237650934256</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -598,10 +592,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>237650988697</t>
-        </is>
+      <c r="A5" t="n">
+        <v>237650988697</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -637,10 +629,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>237651213730</t>
-        </is>
+      <c r="A6" t="n">
+        <v>237651213730</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -676,10 +666,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>237651433330</t>
-        </is>
+      <c r="A7" t="n">
+        <v>237651433330</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -715,10 +703,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>237651533411</t>
-        </is>
+      <c r="A8" t="n">
+        <v>237651533411</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -754,10 +740,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>237651809692</t>
-        </is>
+      <c r="A9" t="n">
+        <v>237651809692</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -793,10 +777,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>237651843112</t>
-        </is>
+      <c r="A10" t="n">
+        <v>237651843112</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -832,10 +814,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>237651927448</t>
-        </is>
+      <c r="A11" t="n">
+        <v>237651927448</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -871,10 +851,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>237651927707</t>
-        </is>
+      <c r="A12" t="n">
+        <v>237651927707</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -910,10 +888,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>237651937677</t>
-        </is>
+      <c r="A13" t="n">
+        <v>237651937677</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -949,10 +925,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>237652194260</t>
-        </is>
+      <c r="A14" t="n">
+        <v>237652194260</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -988,10 +962,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>237652194293</t>
-        </is>
+      <c r="A15" t="n">
+        <v>237652194293</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1027,10 +999,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>237652285489</t>
-        </is>
+      <c r="A16" t="n">
+        <v>237652285489</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1066,10 +1036,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>237652297747</t>
-        </is>
+      <c r="A17" t="n">
+        <v>237652297747</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1105,10 +1073,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>237652427111</t>
-        </is>
+      <c r="A18" t="n">
+        <v>237652427111</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1144,10 +1110,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>237652667691</t>
-        </is>
+      <c r="A19" t="n">
+        <v>237652667691</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1183,10 +1147,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>237652678854</t>
-        </is>
+      <c r="A20" t="n">
+        <v>237652678854</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1222,10 +1184,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>237652807179</t>
-        </is>
+      <c r="A21" t="n">
+        <v>237652807179</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1261,10 +1221,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>237652927180</t>
-        </is>
+      <c r="A22" t="n">
+        <v>237652927180</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1300,10 +1258,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>237652940152</t>
-        </is>
+      <c r="A23" t="n">
+        <v>237652940152</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1339,10 +1295,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>237653294562</t>
-        </is>
+      <c r="A24" t="n">
+        <v>237653294562</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1378,10 +1332,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>237653316656</t>
-        </is>
+      <c r="A25" t="n">
+        <v>237653316656</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1417,10 +1369,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>237653321271</t>
-        </is>
+      <c r="A26" t="n">
+        <v>237653321271</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1456,10 +1406,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>237653430377</t>
-        </is>
+      <c r="A27" t="n">
+        <v>237653430377</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1495,10 +1443,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>237653650087</t>
-        </is>
+      <c r="A28" t="n">
+        <v>237653650087</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1534,10 +1480,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>237653854849</t>
-        </is>
+      <c r="A29" t="n">
+        <v>237653854849</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1573,10 +1517,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>237653901359</t>
-        </is>
+      <c r="A30" t="n">
+        <v>237653901359</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1612,10 +1554,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>237653946894</t>
-        </is>
+      <c r="A31" t="n">
+        <v>237653946894</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1651,10 +1591,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>237653959075</t>
-        </is>
+      <c r="A32" t="n">
+        <v>237653959075</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1690,10 +1628,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>237654137136</t>
-        </is>
+      <c r="A33" t="n">
+        <v>237654137136</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1729,10 +1665,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>237654150202</t>
-        </is>
+      <c r="A34" t="n">
+        <v>237654150202</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1768,10 +1702,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>237654164073</t>
-        </is>
+      <c r="A35" t="n">
+        <v>237654164073</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1807,10 +1739,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>237654247769</t>
-        </is>
+      <c r="A36" t="n">
+        <v>237654247769</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1846,10 +1776,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>237654261990</t>
-        </is>
+      <c r="A37" t="n">
+        <v>237654261990</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1885,10 +1813,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>237654270800</t>
-        </is>
+      <c r="A38" t="n">
+        <v>237654270800</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1924,10 +1850,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>237654355100</t>
-        </is>
+      <c r="A39" t="n">
+        <v>237654355100</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1963,10 +1887,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>237670097580</t>
-        </is>
+      <c r="A40" t="n">
+        <v>237670097580</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -2002,10 +1924,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>237670174030</t>
-        </is>
+      <c r="A41" t="n">
+        <v>237670174030</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -2041,10 +1961,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>237670806337</t>
-        </is>
+      <c r="A42" t="n">
+        <v>237670806337</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -2080,10 +1998,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>237670904526</t>
-        </is>
+      <c r="A43" t="n">
+        <v>237670904526</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -2119,10 +2035,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>237670905160</t>
-        </is>
+      <c r="A44" t="n">
+        <v>237670905160</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -2158,10 +2072,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>237671105715</t>
-        </is>
+      <c r="A45" t="n">
+        <v>237671105715</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -2197,10 +2109,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>237671290825</t>
-        </is>
+      <c r="A46" t="n">
+        <v>237671290825</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -2236,10 +2146,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>237671351291</t>
-        </is>
+      <c r="A47" t="n">
+        <v>237671351291</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -2275,10 +2183,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>237671432720</t>
-        </is>
+      <c r="A48" t="n">
+        <v>237671432720</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -2314,10 +2220,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>237671605749</t>
-        </is>
+      <c r="A49" t="n">
+        <v>237671605749</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -2353,10 +2257,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>237671631547</t>
-        </is>
+      <c r="A50" t="n">
+        <v>237671631547</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -2392,10 +2294,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>237671645947</t>
-        </is>
+      <c r="A51" t="n">
+        <v>237671645947</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -2431,10 +2331,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>237671646117</t>
-        </is>
+      <c r="A52" t="n">
+        <v>237671646117</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -2470,10 +2368,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>237671664239</t>
-        </is>
+      <c r="A53" t="n">
+        <v>237671664239</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -2509,10 +2405,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>237671694408</t>
-        </is>
+      <c r="A54" t="n">
+        <v>237671694408</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -2548,10 +2442,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>237671823369</t>
-        </is>
+      <c r="A55" t="n">
+        <v>237671823369</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -2587,10 +2479,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>237671823371</t>
-        </is>
+      <c r="A56" t="n">
+        <v>237671823371</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -2626,10 +2516,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>237671825253</t>
-        </is>
+      <c r="A57" t="n">
+        <v>237671825253</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -2665,10 +2553,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>237671838460</t>
-        </is>
+      <c r="A58" t="n">
+        <v>237671838460</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -2704,10 +2590,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>237671892536</t>
-        </is>
+      <c r="A59" t="n">
+        <v>237671892536</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -2743,10 +2627,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>237672029564</t>
-        </is>
+      <c r="A60" t="n">
+        <v>237672029564</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -2782,10 +2664,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>237672064755</t>
-        </is>
+      <c r="A61" t="n">
+        <v>237672064755</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -2821,10 +2701,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>237672128028</t>
-        </is>
+      <c r="A62" t="n">
+        <v>237672128028</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -2860,10 +2738,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>237672276931</t>
-        </is>
+      <c r="A63" t="n">
+        <v>237672276931</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -2899,10 +2775,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>237672777139</t>
-        </is>
+      <c r="A64" t="n">
+        <v>237672777139</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -2938,10 +2812,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>237672920086</t>
-        </is>
+      <c r="A65" t="n">
+        <v>237672920086</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -2977,10 +2849,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>237672956746</t>
-        </is>
+      <c r="A66" t="n">
+        <v>237672956746</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -3016,10 +2886,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>237673018936</t>
-        </is>
+      <c r="A67" t="n">
+        <v>237673018936</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -3055,10 +2923,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>237673220938</t>
-        </is>
+      <c r="A68" t="n">
+        <v>237673220938</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -3094,10 +2960,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>237673560726</t>
-        </is>
+      <c r="A69" t="n">
+        <v>237673560726</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -3133,10 +2997,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>237673718583</t>
-        </is>
+      <c r="A70" t="n">
+        <v>237673718583</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -3172,10 +3034,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>237673816350</t>
-        </is>
+      <c r="A71" t="n">
+        <v>237673816350</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -3211,10 +3071,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>237674000053</t>
-        </is>
+      <c r="A72" t="n">
+        <v>237674000053</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -3250,10 +3108,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>237674062440</t>
-        </is>
+      <c r="A73" t="n">
+        <v>237674062440</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -3289,10 +3145,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>237674069453</t>
-        </is>
+      <c r="A74" t="n">
+        <v>237674069453</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -3328,10 +3182,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>237674240552</t>
-        </is>
+      <c r="A75" t="n">
+        <v>237674240552</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -3367,10 +3219,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>237674248126</t>
-        </is>
+      <c r="A76" t="n">
+        <v>237674248126</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -3406,10 +3256,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>237674435926</t>
-        </is>
+      <c r="A77" t="n">
+        <v>237674435926</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -3445,10 +3293,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>237674437082</t>
-        </is>
+      <c r="A78" t="n">
+        <v>237674437082</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -3484,10 +3330,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>237674450580</t>
-        </is>
+      <c r="A79" t="n">
+        <v>237674450580</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -3523,10 +3367,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>237674466307</t>
-        </is>
+      <c r="A80" t="n">
+        <v>237674466307</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -3562,10 +3404,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>237674580187</t>
-        </is>
+      <c r="A81" t="n">
+        <v>237674580187</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -3601,10 +3441,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>237674629681</t>
-        </is>
+      <c r="A82" t="n">
+        <v>237674629681</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -3640,10 +3478,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>237674673359</t>
-        </is>
+      <c r="A83" t="n">
+        <v>237674673359</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -3679,10 +3515,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>237674841555</t>
-        </is>
+      <c r="A84" t="n">
+        <v>237674841555</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -3718,10 +3552,8 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>237674853971</t>
-        </is>
+      <c r="A85" t="n">
+        <v>237674853971</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -3757,10 +3589,8 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>237674884831</t>
-        </is>
+      <c r="A86" t="n">
+        <v>237674884831</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -3796,10 +3626,8 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>237674884916</t>
-        </is>
+      <c r="A87" t="n">
+        <v>237674884916</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -3835,10 +3663,8 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>237674890653</t>
-        </is>
+      <c r="A88" t="n">
+        <v>237674890653</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -3874,10 +3700,8 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>237674892352</t>
-        </is>
+      <c r="A89" t="n">
+        <v>237674892352</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -3913,10 +3737,8 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>237674895078</t>
-        </is>
+      <c r="A90" t="n">
+        <v>237674895078</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -3952,10 +3774,8 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>237674895309</t>
-        </is>
+      <c r="A91" t="n">
+        <v>237674895309</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -3991,10 +3811,8 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>237674895389</t>
-        </is>
+      <c r="A92" t="n">
+        <v>237674895389</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -4030,10 +3848,8 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>237674895877</t>
-        </is>
+      <c r="A93" t="n">
+        <v>237674895877</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -4069,10 +3885,8 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>237674899678</t>
-        </is>
+      <c r="A94" t="n">
+        <v>237674899678</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -4108,10 +3922,8 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>237674929391</t>
-        </is>
+      <c r="A95" t="n">
+        <v>237674929391</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -4147,10 +3959,8 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>237674933048</t>
-        </is>
+      <c r="A96" t="n">
+        <v>237674933048</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -4186,10 +3996,8 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>237674956331</t>
-        </is>
+      <c r="A97" t="n">
+        <v>237674956331</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -4225,10 +4033,8 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>237674979451</t>
-        </is>
+      <c r="A98" t="n">
+        <v>237674979451</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -4264,10 +4070,8 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>237675239360</t>
-        </is>
+      <c r="A99" t="n">
+        <v>237675239360</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -4303,10 +4107,8 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>237675396752</t>
-        </is>
+      <c r="A100" t="n">
+        <v>237675396752</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -4342,10 +4144,8 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>237675432472</t>
-        </is>
+      <c r="A101" t="n">
+        <v>237675432472</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
@@ -4381,10 +4181,8 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>237675443028</t>
-        </is>
+      <c r="A102" t="n">
+        <v>237675443028</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -4420,10 +4218,8 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>237675457527</t>
-        </is>
+      <c r="A103" t="n">
+        <v>237675457527</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -4459,10 +4255,8 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>237675621967</t>
-        </is>
+      <c r="A104" t="n">
+        <v>237675621967</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -4498,10 +4292,8 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>237675641522</t>
-        </is>
+      <c r="A105" t="n">
+        <v>237675641522</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -4537,10 +4329,8 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>237675779272</t>
-        </is>
+      <c r="A106" t="n">
+        <v>237675779272</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -4576,10 +4366,8 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>237675788721</t>
-        </is>
+      <c r="A107" t="n">
+        <v>237675788721</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -4615,10 +4403,8 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>237675831509</t>
-        </is>
+      <c r="A108" t="n">
+        <v>237675831509</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -4654,10 +4440,8 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>237675944533</t>
-        </is>
+      <c r="A109" t="n">
+        <v>237675944533</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -4693,10 +4477,8 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>237675986754</t>
-        </is>
+      <c r="A110" t="n">
+        <v>237675986754</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -4732,10 +4514,8 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>237676036869</t>
-        </is>
+      <c r="A111" t="n">
+        <v>237676036869</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -4771,10 +4551,8 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>237676076193</t>
-        </is>
+      <c r="A112" t="n">
+        <v>237676076193</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -4810,10 +4588,8 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>237676286294</t>
-        </is>
+      <c r="A113" t="n">
+        <v>237676286294</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -4849,10 +4625,8 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>237676301061</t>
-        </is>
+      <c r="A114" t="n">
+        <v>237676301061</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -4888,10 +4662,8 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>237676391673</t>
-        </is>
+      <c r="A115" t="n">
+        <v>237676391673</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -4927,10 +4699,8 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>237676439452</t>
-        </is>
+      <c r="A116" t="n">
+        <v>237676439452</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -4966,10 +4736,8 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>237676575053</t>
-        </is>
+      <c r="A117" t="n">
+        <v>237676575053</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -5005,10 +4773,8 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>237676695935</t>
-        </is>
+      <c r="A118" t="n">
+        <v>237676695935</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -5044,10 +4810,8 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>237676770192</t>
-        </is>
+      <c r="A119" t="n">
+        <v>237676770192</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -5083,10 +4847,8 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>237677178575</t>
-        </is>
+      <c r="A120" t="n">
+        <v>237677178575</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -5122,10 +4884,8 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>237677304210</t>
-        </is>
+      <c r="A121" t="n">
+        <v>237677304210</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -5161,10 +4921,8 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>237677313421</t>
-        </is>
+      <c r="A122" t="n">
+        <v>237677313421</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
@@ -5200,10 +4958,8 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>237677316351</t>
-        </is>
+      <c r="A123" t="n">
+        <v>237677316351</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -5239,10 +4995,8 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>237677525770</t>
-        </is>
+      <c r="A124" t="n">
+        <v>237677525770</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -5278,10 +5032,8 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>237677567788</t>
-        </is>
+      <c r="A125" t="n">
+        <v>237677567788</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -5317,10 +5069,8 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>237677833877</t>
-        </is>
+      <c r="A126" t="n">
+        <v>237677833877</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -5356,10 +5106,8 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>237677880357</t>
-        </is>
+      <c r="A127" t="n">
+        <v>237677880357</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -5395,10 +5143,8 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>237678046498</t>
-        </is>
+      <c r="A128" t="n">
+        <v>237678046498</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
@@ -5434,10 +5180,8 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>237678319711</t>
-        </is>
+      <c r="A129" t="n">
+        <v>237678319711</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -5473,10 +5217,8 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>237678370615</t>
-        </is>
+      <c r="A130" t="n">
+        <v>237678370615</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -5512,10 +5254,8 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>237678384388</t>
-        </is>
+      <c r="A131" t="n">
+        <v>237678384388</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -5551,10 +5291,8 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>237678530662</t>
-        </is>
+      <c r="A132" t="n">
+        <v>237678530662</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -5590,10 +5328,8 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>237678559161</t>
-        </is>
+      <c r="A133" t="n">
+        <v>237678559161</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
@@ -5629,10 +5365,8 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>237678623874</t>
-        </is>
+      <c r="A134" t="n">
+        <v>237678623874</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -5668,10 +5402,8 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>237678637179</t>
-        </is>
+      <c r="A135" t="n">
+        <v>237678637179</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -5707,10 +5439,8 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>237678836319</t>
-        </is>
+      <c r="A136" t="n">
+        <v>237678836319</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -5746,10 +5476,8 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>237678854978</t>
-        </is>
+      <c r="A137" t="n">
+        <v>237678854978</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -5785,10 +5513,8 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>237678872943</t>
-        </is>
+      <c r="A138" t="n">
+        <v>237678872943</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -5824,10 +5550,8 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>237678965562</t>
-        </is>
+      <c r="A139" t="n">
+        <v>237678965562</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
@@ -5863,10 +5587,8 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>237679038720</t>
-        </is>
+      <c r="A140" t="n">
+        <v>237679038720</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
@@ -5902,10 +5624,8 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>237679068456</t>
-        </is>
+      <c r="A141" t="n">
+        <v>237679068456</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
@@ -5941,10 +5661,8 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>237679071551</t>
-        </is>
+      <c r="A142" t="n">
+        <v>237679071551</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
@@ -5980,10 +5698,8 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>237679087694</t>
-        </is>
+      <c r="A143" t="n">
+        <v>237679087694</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -6019,10 +5735,8 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>237679111075</t>
-        </is>
+      <c r="A144" t="n">
+        <v>237679111075</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
@@ -6058,10 +5772,8 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>237679428698</t>
-        </is>
+      <c r="A145" t="n">
+        <v>237679428698</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -6097,10 +5809,8 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>237679551262</t>
-        </is>
+      <c r="A146" t="n">
+        <v>237679551262</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
@@ -6136,10 +5846,8 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>237679553674</t>
-        </is>
+      <c r="A147" t="n">
+        <v>237679553674</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
@@ -6175,10 +5883,8 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>237679580678</t>
-        </is>
+      <c r="A148" t="n">
+        <v>237679580678</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -6214,10 +5920,8 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>237679808809</t>
-        </is>
+      <c r="A149" t="n">
+        <v>237679808809</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
@@ -6253,10 +5957,8 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>237679884264</t>
-        </is>
+      <c r="A150" t="n">
+        <v>237679884264</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -6292,10 +5994,8 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>237680116452</t>
-        </is>
+      <c r="A151" t="n">
+        <v>237680116452</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
@@ -6331,10 +6031,8 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>237680119435</t>
-        </is>
+      <c r="A152" t="n">
+        <v>237680119435</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
@@ -6370,10 +6068,8 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>237680144977</t>
-        </is>
+      <c r="A153" t="n">
+        <v>237680144977</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
@@ -6409,10 +6105,8 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>237680435802</t>
-        </is>
+      <c r="A154" t="n">
+        <v>237680435802</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
@@ -6448,10 +6142,8 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>237680472978</t>
-        </is>
+      <c r="A155" t="n">
+        <v>237680472978</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
@@ -6487,10 +6179,8 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>237680574202</t>
-        </is>
+      <c r="A156" t="n">
+        <v>237680574202</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -6526,10 +6216,8 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>237680670799</t>
-        </is>
+      <c r="A157" t="n">
+        <v>237680670799</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
@@ -6565,10 +6253,8 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>237680857383</t>
-        </is>
+      <c r="A158" t="n">
+        <v>237680857383</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
@@ -6604,10 +6290,8 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>237680943213</t>
-        </is>
+      <c r="A159" t="n">
+        <v>237680943213</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -6643,10 +6327,8 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>237681019523</t>
-        </is>
+      <c r="A160" t="n">
+        <v>237681019523</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -6682,10 +6364,8 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>237681114247</t>
-        </is>
+      <c r="A161" t="n">
+        <v>237681114247</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -6721,10 +6401,8 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>237681118330</t>
-        </is>
+      <c r="A162" t="n">
+        <v>237681118330</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
@@ -6760,10 +6438,8 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>237681299829</t>
-        </is>
+      <c r="A163" t="n">
+        <v>237681299829</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -6799,10 +6475,8 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>237681602244</t>
-        </is>
+      <c r="A164" t="n">
+        <v>237681602244</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -6838,10 +6512,8 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>237681603496</t>
-        </is>
+      <c r="A165" t="n">
+        <v>237681603496</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -6877,10 +6549,8 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>237681655241</t>
-        </is>
+      <c r="A166" t="n">
+        <v>237681655241</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -6916,10 +6586,8 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>237681657614</t>
-        </is>
+      <c r="A167" t="n">
+        <v>237681657614</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -6955,10 +6623,8 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>237681657939</t>
-        </is>
+      <c r="A168" t="n">
+        <v>237681657939</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -6994,10 +6660,8 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>237681662596</t>
-        </is>
+      <c r="A169" t="n">
+        <v>237681662596</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -7033,10 +6697,8 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>237681662606</t>
-        </is>
+      <c r="A170" t="n">
+        <v>237681662606</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -7072,10 +6734,8 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>237681662680</t>
-        </is>
+      <c r="A171" t="n">
+        <v>237681662680</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
@@ -7111,10 +6771,8 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>237681678622</t>
-        </is>
+      <c r="A172" t="n">
+        <v>237681678622</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -7150,10 +6808,8 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>237681679096</t>
-        </is>
+      <c r="A173" t="n">
+        <v>237681679096</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
@@ -7189,10 +6845,8 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>237681862876</t>
-        </is>
+      <c r="A174" t="n">
+        <v>237681862876</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
@@ -7228,10 +6882,8 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>237682117915</t>
-        </is>
+      <c r="A175" t="n">
+        <v>237682117915</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
@@ -7267,10 +6919,8 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>237682154553</t>
-        </is>
+      <c r="A176" t="n">
+        <v>237682154553</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -7306,10 +6956,8 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>237682238745</t>
-        </is>
+      <c r="A177" t="n">
+        <v>237682238745</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
@@ -7345,10 +6993,8 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>237682316602</t>
-        </is>
+      <c r="A178" t="n">
+        <v>237682316602</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -7384,10 +7030,8 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>237682368679</t>
-        </is>
+      <c r="A179" t="n">
+        <v>237682368679</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
@@ -7423,10 +7067,8 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>237682370358</t>
-        </is>
+      <c r="A180" t="n">
+        <v>237682370358</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
@@ -7462,10 +7104,8 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>237682480811</t>
-        </is>
+      <c r="A181" t="n">
+        <v>237682480811</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
@@ -7501,10 +7141,8 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>237682612277</t>
-        </is>
+      <c r="A182" t="n">
+        <v>237682612277</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
@@ -7540,10 +7178,8 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>237682639044</t>
-        </is>
+      <c r="A183" t="n">
+        <v>237682639044</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
@@ -7579,10 +7215,8 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>237683023087</t>
-        </is>
+      <c r="A184" t="n">
+        <v>237683023087</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
@@ -7618,10 +7252,8 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" t="inlineStr">
-        <is>
-          <t>237683368985</t>
-        </is>
+      <c r="A185" t="n">
+        <v>237683368985</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
@@ -7657,10 +7289,8 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" t="inlineStr">
-        <is>
-          <t>237683379070</t>
-        </is>
+      <c r="A186" t="n">
+        <v>237683379070</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
@@ -7696,10 +7326,8 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" t="inlineStr">
-        <is>
-          <t>237683379155</t>
-        </is>
+      <c r="A187" t="n">
+        <v>237683379155</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
@@ -7735,10 +7363,8 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" t="inlineStr">
-        <is>
-          <t>237683386020</t>
-        </is>
+      <c r="A188" t="n">
+        <v>237683386020</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
@@ -7774,10 +7400,8 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" t="inlineStr">
-        <is>
-          <t>237683396173</t>
-        </is>
+      <c r="A189" t="n">
+        <v>237683396173</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
@@ -7813,10 +7437,8 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t>237683400719</t>
-        </is>
+      <c r="A190" t="n">
+        <v>237683400719</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
@@ -7852,10 +7474,8 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" t="inlineStr">
-        <is>
-          <t>237683408221</t>
-        </is>
+      <c r="A191" t="n">
+        <v>237683408221</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
@@ -7891,10 +7511,8 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" t="inlineStr">
-        <is>
-          <t>237683555873</t>
-        </is>
+      <c r="A192" t="n">
+        <v>237683555873</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
@@ -7930,10 +7548,8 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" t="inlineStr">
-        <is>
-          <t>237683730580</t>
-        </is>
+      <c r="A193" t="n">
+        <v>237683730580</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update project files and fix streamlit version conflict
</commit_message>
<xml_diff>
--- a/reconciliation.xlsx
+++ b/reconciliation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="192">
   <si>
     <t>Numero</t>
   </si>
@@ -527,6 +527,18 @@
   </si>
   <si>
     <t>YVETTE LAURE NGANDO SIMO EPSE DIMO</t>
+  </si>
+  <si>
+    <t>BEATRICE TCHAMTIEU EPSE NGAMENI</t>
+  </si>
+  <si>
+    <t>VIVIANE MADJUIMEKEM FOMEKONG</t>
+  </si>
+  <si>
+    <t>SAGNOU BRINDA JOSELINE _DIGITAL BUSINESS SARL</t>
+  </si>
+  <si>
+    <t>MFS MAKEPE MATURITE</t>
   </si>
   <si>
     <t>Rte_0</t>
@@ -935,7 +947,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -978,10 +990,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E2">
         <v>19150</v>
@@ -996,7 +1008,7 @@
         <v>1.415770234986945</v>
       </c>
       <c r="I2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1007,10 +1019,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E3">
         <v>5000</v>
@@ -1025,7 +1037,7 @@
         <v>3.0728</v>
       </c>
       <c r="I3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1036,10 +1048,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E4">
         <v>84390</v>
@@ -1054,7 +1066,7 @@
         <v>0.1093731484773077</v>
       </c>
       <c r="I4" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1065,10 +1077,10 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D5" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E5">
         <v>260865</v>
@@ -1083,7 +1095,7 @@
         <v>2.685546163724532</v>
       </c>
       <c r="I5" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1094,10 +1106,10 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E6">
         <v>28141.53846153846</v>
@@ -1112,7 +1124,7 @@
         <v>1.233443581893724</v>
       </c>
       <c r="I6" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1123,10 +1135,10 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D7" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E7">
         <v>38670</v>
@@ -1141,7 +1153,7 @@
         <v>17.1059219032842</v>
       </c>
       <c r="I7" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1152,10 +1164,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E8">
         <v>46826</v>
@@ -1170,7 +1182,7 @@
         <v>0.4723871353521548</v>
       </c>
       <c r="I8" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1181,10 +1193,10 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D9" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E9">
         <v>14676.42857142857</v>
@@ -1199,7 +1211,7 @@
         <v>5.942658295614932</v>
       </c>
       <c r="I9" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1210,10 +1222,10 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D10" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E10">
         <v>13250</v>
@@ -1228,7 +1240,7 @@
         <v>0.6353207547169811</v>
       </c>
       <c r="I10" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1239,10 +1251,10 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E11">
         <v>8935.719999999999</v>
@@ -1257,7 +1269,7 @@
         <v>1.570326733604007</v>
       </c>
       <c r="I11" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1268,10 +1280,10 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D12" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E12">
         <v>223404</v>
@@ -1286,7 +1298,7 @@
         <v>1.613655082272475</v>
       </c>
       <c r="I12" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1297,10 +1309,10 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E13">
         <v>5493.333333333333</v>
@@ -1315,7 +1327,7 @@
         <v>2.123118932038835</v>
       </c>
       <c r="I13" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1326,10 +1338,10 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D14" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E14">
         <v>284192.6444444444</v>
@@ -1344,7 +1356,7 @@
         <v>0.147498539527452</v>
       </c>
       <c r="I14" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1355,10 +1367,10 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D15" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E15">
         <v>7220</v>
@@ -1373,7 +1385,7 @@
         <v>3.068975069252077</v>
       </c>
       <c r="I15" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1384,10 +1396,10 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D16" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E16">
         <v>38878.39000000001</v>
@@ -1402,7 +1414,7 @@
         <v>1.854397777274213</v>
       </c>
       <c r="I16" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1413,10 +1425,10 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D17" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E17">
         <v>7380.523076923077</v>
@@ -1431,7 +1443,7 @@
         <v>0.5148686563804108</v>
       </c>
       <c r="I17" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1442,10 +1454,10 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E18">
         <v>26419.66666666666</v>
@@ -1460,7 +1472,7 @@
         <v>0.9661741884202428</v>
       </c>
       <c r="I18" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1471,10 +1483,10 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D19" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E19">
         <v>39192.5</v>
@@ -1489,7 +1501,7 @@
         <v>0.006174650762263188</v>
       </c>
       <c r="I19" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1500,10 +1512,10 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E20">
         <v>333240</v>
@@ -1518,7 +1530,7 @@
         <v>0.940406313767855</v>
       </c>
       <c r="I20" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1529,10 +1541,10 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E21">
         <v>62720</v>
@@ -1547,7 +1559,7 @@
         <v>4.549250637755102</v>
       </c>
       <c r="I21" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1558,10 +1570,10 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E22">
         <v>38170</v>
@@ -1576,7 +1588,7 @@
         <v>6.635472884464239</v>
       </c>
       <c r="I22" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1587,10 +1599,10 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D23" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E23">
         <v>172860</v>
@@ -1605,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1616,10 +1628,10 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E24">
         <v>53438.45714285715</v>
@@ -1634,7 +1646,7 @@
         <v>1.492913610636748</v>
       </c>
       <c r="I24" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1645,10 +1657,10 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D25" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E25">
         <v>55864.54545454546</v>
@@ -1663,7 +1675,7 @@
         <v>2.86292493205969</v>
       </c>
       <c r="I25" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1674,10 +1686,10 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D26" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E26">
         <v>18750</v>
@@ -1692,7 +1704,7 @@
         <v>0.8024</v>
       </c>
       <c r="I26" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1703,10 +1715,10 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D27" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E27">
         <v>14265</v>
@@ -1721,7 +1733,7 @@
         <v>2.024956186470382</v>
       </c>
       <c r="I27" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1732,10 +1744,10 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D28" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E28">
         <v>271168</v>
@@ -1750,7 +1762,7 @@
         <v>0.4647119129100779</v>
       </c>
       <c r="I28" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1761,10 +1773,10 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D29" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E29">
         <v>35537.4</v>
@@ -1779,7 +1791,7 @@
         <v>0.6158300832362524</v>
       </c>
       <c r="I29" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1790,10 +1802,10 @@
         <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D30" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E30">
         <v>195936.25</v>
@@ -1808,7 +1820,7 @@
         <v>1.659478529368609</v>
       </c>
       <c r="I30" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1819,10 +1831,10 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D31" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E31">
         <v>136459.0909090909</v>
@@ -1837,7 +1849,7 @@
         <v>2.140524299656907</v>
       </c>
       <c r="I31" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1848,10 +1860,10 @@
         <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D32" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E32">
         <v>159153.3333333333</v>
@@ -1866,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1877,10 +1889,10 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D33" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E33">
         <v>41870</v>
@@ -1895,7 +1907,7 @@
         <v>0.03694769524719369</v>
       </c>
       <c r="I33" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1906,10 +1918,10 @@
         <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D34" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E34">
         <v>235988.3333333334</v>
@@ -1924,7 +1936,7 @@
         <v>0.1087935138036485</v>
       </c>
       <c r="I34" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1935,10 +1947,10 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D35" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E35">
         <v>39758.21666666667</v>
@@ -1953,7 +1965,7 @@
         <v>0.7710858929370156</v>
       </c>
       <c r="I35" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1964,10 +1976,10 @@
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D36" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E36">
         <v>74657.14285714286</v>
@@ -1982,7 +1994,7 @@
         <v>4.457577497129736</v>
       </c>
       <c r="I36" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1993,10 +2005,10 @@
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D37" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E37">
         <v>500000</v>
@@ -2011,7 +2023,7 @@
         <v>0.389164</v>
       </c>
       <c r="I37" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2022,10 +2034,10 @@
         <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D38" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E38">
         <v>113235</v>
@@ -2040,7 +2052,7 @@
         <v>0.6954386894511414</v>
       </c>
       <c r="I38" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2051,10 +2063,10 @@
         <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D39" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E39">
         <v>90695</v>
@@ -2069,7 +2081,7 @@
         <v>6.502001212856277</v>
       </c>
       <c r="I39" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2080,10 +2092,10 @@
         <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D40" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E40">
         <v>176790</v>
@@ -2098,7 +2110,7 @@
         <v>0.06353300526047853</v>
       </c>
       <c r="I40" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2109,10 +2121,10 @@
         <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D41" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E41">
         <v>15660</v>
@@ -2127,7 +2139,7 @@
         <v>8.755938697318008</v>
       </c>
       <c r="I41" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2138,10 +2150,10 @@
         <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D42" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E42">
         <v>28554.8</v>
@@ -2156,7 +2168,7 @@
         <v>1.325241290431031</v>
       </c>
       <c r="I42" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2167,10 +2179,10 @@
         <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D43" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E43">
         <v>34912.72727272727</v>
@@ -2185,7 +2197,7 @@
         <v>3.012798146026455</v>
       </c>
       <c r="I43" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2196,10 +2208,10 @@
         <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D44" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E44">
         <v>96559.8</v>
@@ -2214,7 +2226,7 @@
         <v>6.712462121918231</v>
       </c>
       <c r="I44" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2225,10 +2237,10 @@
         <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D45" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E45">
         <v>129030</v>
@@ -2243,7 +2255,7 @@
         <v>1.180477408354646</v>
       </c>
       <c r="I45" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2254,10 +2266,10 @@
         <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D46" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E46">
         <v>145740</v>
@@ -2272,7 +2284,7 @@
         <v>1.070522848909016</v>
       </c>
       <c r="I46" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2283,10 +2295,10 @@
         <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D47" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E47">
         <v>31576.24</v>
@@ -2301,7 +2313,7 @@
         <v>2.552647180284923</v>
       </c>
       <c r="I47" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2312,10 +2324,10 @@
         <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D48" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E48">
         <v>54855.31111111111</v>
@@ -2330,7 +2342,7 @@
         <v>0.9403282736929353</v>
       </c>
       <c r="I48" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2341,10 +2353,10 @@
         <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D49" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E49">
         <v>30030</v>
@@ -2359,7 +2371,7 @@
         <v>12.5002664002664</v>
       </c>
       <c r="I49" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2370,10 +2382,10 @@
         <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D50" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E50">
         <v>18795</v>
@@ -2388,7 +2400,7 @@
         <v>14.79318967810588</v>
       </c>
       <c r="I50" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2399,10 +2411,10 @@
         <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D51" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E51">
         <v>48162</v>
@@ -2417,7 +2429,7 @@
         <v>8.494165524687514</v>
       </c>
       <c r="I51" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2428,10 +2440,10 @@
         <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D52" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E52">
         <v>41275.71428571428</v>
@@ -2446,7 +2458,7 @@
         <v>4.615232063129478</v>
       </c>
       <c r="I52" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2457,10 +2469,10 @@
         <v>60</v>
       </c>
       <c r="C53" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D53" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E53">
         <v>30923.33333333334</v>
@@ -2475,7 +2487,7 @@
         <v>1.096388918831519</v>
       </c>
       <c r="I53" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2486,10 +2498,10 @@
         <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D54" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E54">
         <v>86783.84615384616</v>
@@ -2504,7 +2516,7 @@
         <v>0.006579565498719187</v>
       </c>
       <c r="I54" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2515,10 +2527,10 @@
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D55" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E55">
         <v>328228.8</v>
@@ -2533,7 +2545,7 @@
         <v>0.01132137094612051</v>
       </c>
       <c r="I55" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2544,10 +2556,10 @@
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D56" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E56">
         <v>85360</v>
@@ -2562,7 +2574,7 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2573,10 +2585,10 @@
         <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D57" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E57">
         <v>103179.8</v>
@@ -2591,7 +2603,7 @@
         <v>4.278831709307441</v>
       </c>
       <c r="I57" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2602,10 +2614,10 @@
         <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D58" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E58">
         <v>178497.5</v>
@@ -2620,7 +2632,7 @@
         <v>3.279889074076668</v>
       </c>
       <c r="I58" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2631,10 +2643,10 @@
         <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D59" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E59">
         <v>500000</v>
@@ -2649,7 +2661,7 @@
         <v>0.65001</v>
       </c>
       <c r="I59" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2660,10 +2672,10 @@
         <v>67</v>
       </c>
       <c r="C60" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D60" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E60">
         <v>6183.636363636364</v>
@@ -2678,7 +2690,7 @@
         <v>0.5162011173184358</v>
       </c>
       <c r="I60" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2689,10 +2701,10 @@
         <v>68</v>
       </c>
       <c r="C61" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D61" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E61">
         <v>114838.4615384615</v>
@@ -2707,7 +2719,7 @@
         <v>1.08703128139862</v>
       </c>
       <c r="I61" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2718,10 +2730,10 @@
         <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D62" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E62">
         <v>29820</v>
@@ -2736,7 +2748,7 @@
         <v>12.70107310529846</v>
       </c>
       <c r="I62" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2747,10 +2759,10 @@
         <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D63" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E63">
         <v>145105</v>
@@ -2765,7 +2777,7 @@
         <v>4.746397436339203</v>
       </c>
       <c r="I63" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2776,10 +2788,10 @@
         <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D64" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E64">
         <v>242106.6666666666</v>
@@ -2794,7 +2806,7 @@
         <v>3.094706190109043</v>
       </c>
       <c r="I64" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2805,10 +2817,10 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D65" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E65">
         <v>23150</v>
@@ -2823,7 +2835,7 @@
         <v>6.186522678185745</v>
       </c>
       <c r="I65" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2834,10 +2846,10 @@
         <v>73</v>
       </c>
       <c r="C66" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D66" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E66">
         <v>43130</v>
@@ -2852,7 +2864,7 @@
         <v>10.75998145142592</v>
       </c>
       <c r="I66" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2863,10 +2875,10 @@
         <v>74</v>
       </c>
       <c r="C67" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D67" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E67">
         <v>7120</v>
@@ -2881,7 +2893,7 @@
         <v>6.41376404494382</v>
       </c>
       <c r="I67" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2892,10 +2904,10 @@
         <v>75</v>
       </c>
       <c r="C68" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D68" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E68">
         <v>12128.57142857143</v>
@@ -2910,7 +2922,7 @@
         <v>5.23243816254417</v>
       </c>
       <c r="I68" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2921,10 +2933,10 @@
         <v>76</v>
       </c>
       <c r="C69" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D69" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E69">
         <v>75599.88333333333</v>
@@ -2939,7 +2951,7 @@
         <v>2.552940447659421</v>
       </c>
       <c r="I69" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2950,10 +2962,10 @@
         <v>77</v>
       </c>
       <c r="C70" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D70" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E70">
         <v>239424</v>
@@ -2968,7 +2980,7 @@
         <v>0.001791800320769848</v>
       </c>
       <c r="I70" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2979,10 +2991,10 @@
         <v>78</v>
       </c>
       <c r="C71" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D71" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E71">
         <v>79250</v>
@@ -2997,7 +3009,7 @@
         <v>2.946965299684543</v>
       </c>
       <c r="I71" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -3008,10 +3020,10 @@
         <v>79</v>
       </c>
       <c r="C72" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D72" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E72">
         <v>118868</v>
@@ -3026,7 +3038,7 @@
         <v>0.9735000168253861</v>
       </c>
       <c r="I72" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3037,10 +3049,10 @@
         <v>80</v>
       </c>
       <c r="C73" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D73" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E73">
         <v>137844.9629629629</v>
@@ -3055,7 +3067,7 @@
         <v>0.02645000529311782</v>
       </c>
       <c r="I73" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3066,10 +3078,10 @@
         <v>81</v>
       </c>
       <c r="C74" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D74" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E74">
         <v>5000</v>
@@ -3084,7 +3096,7 @@
         <v>0.0008</v>
       </c>
       <c r="I74" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -3095,10 +3107,10 @@
         <v>82</v>
       </c>
       <c r="C75" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D75" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E75">
         <v>15997.69230769231</v>
@@ -3113,7 +3125,7 @@
         <v>6.787854017406357</v>
       </c>
       <c r="I75" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -3124,10 +3136,10 @@
         <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D76" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E76">
         <v>28041.81818181818</v>
@@ -3142,7 +3154,7 @@
         <v>4.932383453284056</v>
       </c>
       <c r="I76" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -3153,10 +3165,10 @@
         <v>84</v>
       </c>
       <c r="C77" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D77" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E77">
         <v>14380</v>
@@ -3171,7 +3183,7 @@
         <v>4.255146036161335</v>
       </c>
       <c r="I77" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3182,10 +3194,10 @@
         <v>85</v>
       </c>
       <c r="C78" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D78" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E78">
         <v>12800</v>
@@ -3200,7 +3212,7 @@
         <v>1.9940625</v>
       </c>
       <c r="I78" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -3211,10 +3223,10 @@
         <v>86</v>
       </c>
       <c r="C79" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D79" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E79">
         <v>190430</v>
@@ -3229,7 +3241,7 @@
         <v>2.090999317334453</v>
       </c>
       <c r="I79" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -3240,10 +3252,10 @@
         <v>87</v>
       </c>
       <c r="C80" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D80" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E80">
         <v>5327.599999999999</v>
@@ -3258,7 +3270,7 @@
         <v>0.9644117426233202</v>
       </c>
       <c r="I80" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3269,10 +3281,10 @@
         <v>88</v>
       </c>
       <c r="C81" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D81" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E81">
         <v>27650</v>
@@ -3287,7 +3299,7 @@
         <v>14.92723327305606</v>
       </c>
       <c r="I81" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3298,10 +3310,10 @@
         <v>89</v>
       </c>
       <c r="C82" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D82" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E82">
         <v>112594</v>
@@ -3316,7 +3328,7 @@
         <v>1.871245359433007</v>
       </c>
       <c r="I82" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3327,10 +3339,10 @@
         <v>90</v>
       </c>
       <c r="C83" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D83" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E83">
         <v>108762.35</v>
@@ -3345,7 +3357,7 @@
         <v>6.313370389661496</v>
       </c>
       <c r="I83" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3356,10 +3368,10 @@
         <v>91</v>
       </c>
       <c r="C84" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D84" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E84">
         <v>20715.26153846153</v>
@@ -3374,7 +3386,7 @@
         <v>1.687644635096236</v>
       </c>
       <c r="I84" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3385,10 +3397,10 @@
         <v>92</v>
       </c>
       <c r="C85" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D85" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E85">
         <v>34610</v>
@@ -3403,7 +3415,7 @@
         <v>5.895088124819416</v>
       </c>
       <c r="I85" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3414,10 +3426,10 @@
         <v>93</v>
       </c>
       <c r="C86" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D86" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E86">
         <v>189785.8</v>
@@ -3432,7 +3444,7 @@
         <v>0.5829361311541749</v>
       </c>
       <c r="I86" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3443,10 +3455,10 @@
         <v>94</v>
       </c>
       <c r="C87" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D87" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E87">
         <v>25030</v>
@@ -3461,7 +3473,7 @@
         <v>0.8982421094686376</v>
       </c>
       <c r="I87" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3472,10 +3484,10 @@
         <v>95</v>
       </c>
       <c r="C88" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D88" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E88">
         <v>26250</v>
@@ -3490,7 +3502,7 @@
         <v>27.69318095238095</v>
       </c>
       <c r="I88" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3501,10 +3513,10 @@
         <v>96</v>
       </c>
       <c r="C89" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D89" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E89">
         <v>182169.7</v>
@@ -3519,7 +3531,7 @@
         <v>0.7091684292173726</v>
       </c>
       <c r="I89" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3530,10 +3542,10 @@
         <v>97</v>
       </c>
       <c r="C90" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D90" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E90">
         <v>5000</v>
@@ -3548,7 +3560,7 @@
         <v>3.021</v>
       </c>
       <c r="I90" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3559,10 +3571,10 @@
         <v>98</v>
       </c>
       <c r="C91" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D91" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E91">
         <v>184162.0370370371</v>
@@ -3577,7 +3589,7 @@
         <v>0.1561613916890822</v>
       </c>
       <c r="I91" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3588,10 +3600,10 @@
         <v>99</v>
       </c>
       <c r="C92" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D92" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E92">
         <v>61193.33333333334</v>
@@ -3606,7 +3618,7 @@
         <v>2.240080618803791</v>
       </c>
       <c r="I92" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -3617,10 +3629,10 @@
         <v>100</v>
       </c>
       <c r="C93" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D93" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E93">
         <v>16520</v>
@@ -3635,7 +3647,7 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -3646,10 +3658,10 @@
         <v>101</v>
       </c>
       <c r="C94" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D94" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E94">
         <v>100229.8</v>
@@ -3664,7 +3676,7 @@
         <v>2.388171980788149</v>
       </c>
       <c r="I94" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3675,10 +3687,10 @@
         <v>102</v>
       </c>
       <c r="C95" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D95" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E95">
         <v>25619.09090909091</v>
@@ -3693,7 +3705,7 @@
         <v>3.703449132394166</v>
       </c>
       <c r="I95" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3704,10 +3716,10 @@
         <v>103</v>
       </c>
       <c r="C96" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D96" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E96">
         <v>56220</v>
@@ -3722,7 +3734,7 @@
         <v>21.2746709356101</v>
       </c>
       <c r="I96" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3733,10 +3745,10 @@
         <v>104</v>
       </c>
       <c r="C97" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D97" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E97">
         <v>59610</v>
@@ -3751,7 +3763,7 @@
         <v>1.111675893306492</v>
       </c>
       <c r="I97" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3762,10 +3774,10 @@
         <v>105</v>
       </c>
       <c r="C98" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D98" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E98">
         <v>57805.71428571429</v>
@@ -3780,7 +3792,7 @@
         <v>2.296018683274021</v>
       </c>
       <c r="I98" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3791,10 +3803,10 @@
         <v>106</v>
       </c>
       <c r="C99" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D99" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E99">
         <v>47813.75</v>
@@ -3809,7 +3821,7 @@
         <v>10.42812998352984</v>
       </c>
       <c r="I99" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3820,10 +3832,10 @@
         <v>107</v>
       </c>
       <c r="C100" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D100" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E100">
         <v>7438.090909090909</v>
@@ -3838,7 +3850,7 @@
         <v>2.035871863503587</v>
       </c>
       <c r="I100" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3849,10 +3861,10 @@
         <v>108</v>
       </c>
       <c r="C101" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D101" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E101">
         <v>123740</v>
@@ -3867,7 +3879,7 @@
         <v>2.202998222078552</v>
       </c>
       <c r="I101" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -3878,10 +3890,10 @@
         <v>109</v>
       </c>
       <c r="C102" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D102" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E102">
         <v>7776.875</v>
@@ -3896,7 +3908,7 @@
         <v>5.046242867475689</v>
       </c>
       <c r="I102" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -3907,10 +3919,10 @@
         <v>110</v>
       </c>
       <c r="C103" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D103" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E103">
         <v>47969.93333333333</v>
@@ -3925,7 +3937,7 @@
         <v>6.458086940569719</v>
       </c>
       <c r="I103" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -3936,10 +3948,10 @@
         <v>111</v>
       </c>
       <c r="C104" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D104" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E104">
         <v>107070</v>
@@ -3954,7 +3966,7 @@
         <v>5.532614177640796</v>
       </c>
       <c r="I104" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -3965,10 +3977,10 @@
         <v>112</v>
       </c>
       <c r="C105" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D105" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E105">
         <v>5000</v>
@@ -3983,7 +3995,7 @@
         <v>0.6798</v>
       </c>
       <c r="I105" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -3994,10 +4006,10 @@
         <v>113</v>
       </c>
       <c r="C106" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D106" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E106">
         <v>40660</v>
@@ -4012,7 +4024,7 @@
         <v>31.34419576979833</v>
       </c>
       <c r="I106" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -4023,10 +4035,10 @@
         <v>114</v>
       </c>
       <c r="C107" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D107" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E107">
         <v>26953.63636363636</v>
@@ -4041,7 +4053,7 @@
         <v>1.290920435765119</v>
       </c>
       <c r="I107" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -4052,10 +4064,10 @@
         <v>115</v>
       </c>
       <c r="C108" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D108" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E108">
         <v>45439.84</v>
@@ -4070,7 +4082,7 @@
         <v>0.1198947883619309</v>
       </c>
       <c r="I108" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -4081,10 +4093,10 @@
         <v>116</v>
       </c>
       <c r="C109" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D109" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E109">
         <v>54767.77777777778</v>
@@ -4099,7 +4111,7 @@
         <v>0.03613438558763263</v>
       </c>
       <c r="I109" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -4110,10 +4122,10 @@
         <v>117</v>
       </c>
       <c r="C110" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D110" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E110">
         <v>80918.93000000001</v>
@@ -4128,7 +4140,7 @@
         <v>6.77183942002199</v>
       </c>
       <c r="I110" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -4139,10 +4151,10 @@
         <v>118</v>
       </c>
       <c r="C111" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D111" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E111">
         <v>500000</v>
@@ -4157,7 +4169,7 @@
         <v>7.77873</v>
       </c>
       <c r="I111" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -4168,10 +4180,10 @@
         <v>119</v>
       </c>
       <c r="C112" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D112" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E112">
         <v>60430</v>
@@ -4186,7 +4198,7 @@
         <v>0.9120304484527553</v>
       </c>
       <c r="I112" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -4197,10 +4209,10 @@
         <v>120</v>
       </c>
       <c r="C113" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D113" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E113">
         <v>27020</v>
@@ -4215,7 +4227,7 @@
         <v>6.647964470762398</v>
       </c>
       <c r="I113" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -4226,10 +4238,10 @@
         <v>121</v>
       </c>
       <c r="C114" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D114" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E114">
         <v>5000</v>
@@ -4244,7 +4256,7 @@
         <v>4.0858</v>
       </c>
       <c r="I114" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -4255,10 +4267,10 @@
         <v>122</v>
       </c>
       <c r="C115" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D115" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E115">
         <v>16698.33333333333</v>
@@ -4273,7 +4285,7 @@
         <v>2.710150713644076</v>
       </c>
       <c r="I115" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -4284,10 +4296,10 @@
         <v>123</v>
       </c>
       <c r="C116" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D116" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E116">
         <v>25916.63076923077</v>
@@ -4302,7 +4314,7 @@
         <v>0.8909337099254948</v>
       </c>
       <c r="I116" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -4313,10 +4325,10 @@
         <v>124</v>
       </c>
       <c r="C117" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D117" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E117">
         <v>8800</v>
@@ -4331,7 +4343,7 @@
         <v>2.306931818181818</v>
       </c>
       <c r="I117" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -4342,10 +4354,10 @@
         <v>125</v>
       </c>
       <c r="C118" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D118" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E118">
         <v>43870</v>
@@ -4360,7 +4372,7 @@
         <v>2.031000683838614</v>
       </c>
       <c r="I118" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -4371,10 +4383,10 @@
         <v>126</v>
       </c>
       <c r="C119" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D119" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E119">
         <v>233104.6</v>
@@ -4389,7 +4401,7 @@
         <v>1.486843245478639</v>
       </c>
       <c r="I119" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="120" spans="1:9">
@@ -4400,10 +4412,10 @@
         <v>127</v>
       </c>
       <c r="C120" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D120" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E120">
         <v>149646.6666666667</v>
@@ -4418,7 +4430,7 @@
         <v>6.584991312870316</v>
       </c>
       <c r="I120" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -4429,10 +4441,10 @@
         <v>128</v>
       </c>
       <c r="C121" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D121" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E121">
         <v>500000</v>
@@ -4447,7 +4459,7 @@
         <v>5.523966</v>
       </c>
       <c r="I121" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -4458,10 +4470,10 @@
         <v>129</v>
       </c>
       <c r="C122" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D122" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E122">
         <v>12360.93333333334</v>
@@ -4476,7 +4488,7 @@
         <v>4.262865803013796</v>
       </c>
       <c r="I122" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -4487,10 +4499,10 @@
         <v>130</v>
       </c>
       <c r="C123" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D123" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E123">
         <v>94100</v>
@@ -4505,7 +4517,7 @@
         <v>5.242189160467587</v>
       </c>
       <c r="I123" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -4516,10 +4528,10 @@
         <v>131</v>
       </c>
       <c r="C124" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D124" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E124">
         <v>169880</v>
@@ -4534,7 +4546,7 @@
         <v>10.42050270779374</v>
       </c>
       <c r="I124" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -4545,10 +4557,10 @@
         <v>132</v>
       </c>
       <c r="C125" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D125" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E125">
         <v>7700</v>
@@ -4563,7 +4575,7 @@
         <v>2.328831168831169</v>
       </c>
       <c r="I125" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -4574,10 +4586,10 @@
         <v>133</v>
       </c>
       <c r="C126" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D126" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E126">
         <v>88440</v>
@@ -4592,7 +4604,7 @@
         <v>11.27762324739937</v>
       </c>
       <c r="I126" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -4603,10 +4615,10 @@
         <v>134</v>
       </c>
       <c r="C127" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D127" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E127">
         <v>27588.26086956522</v>
@@ -4621,7 +4633,7 @@
         <v>1.166510645674751</v>
       </c>
       <c r="I127" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="128" spans="1:9">
@@ -4632,10 +4644,10 @@
         <v>135</v>
       </c>
       <c r="C128" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D128" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E128">
         <v>104380</v>
@@ -4650,7 +4662,7 @@
         <v>1.5195822954589</v>
       </c>
       <c r="I128" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -4661,10 +4673,10 @@
         <v>136</v>
       </c>
       <c r="C129" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D129" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E129">
         <v>173354.6</v>
@@ -4679,7 +4691,7 @@
         <v>1.093423537650573</v>
       </c>
       <c r="I129" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -4690,10 +4702,10 @@
         <v>137</v>
       </c>
       <c r="C130" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D130" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E130">
         <v>112810</v>
@@ -4708,7 +4720,7 @@
         <v>0.2139172059214609</v>
       </c>
       <c r="I130" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -4719,10 +4731,10 @@
         <v>138</v>
       </c>
       <c r="C131" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D131" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E131">
         <v>140210</v>
@@ -4737,7 +4749,7 @@
         <v>2.473896298409529</v>
       </c>
       <c r="I131" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -4748,10 +4760,10 @@
         <v>139</v>
       </c>
       <c r="C132" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D132" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E132">
         <v>55020</v>
@@ -4766,7 +4778,7 @@
         <v>0.5756997455470738</v>
       </c>
       <c r="I132" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -4777,10 +4789,10 @@
         <v>140</v>
       </c>
       <c r="C133" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D133" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E133">
         <v>22670</v>
@@ -4795,7 +4807,7 @@
         <v>4.01005734450816</v>
       </c>
       <c r="I133" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -4806,10 +4818,10 @@
         <v>141</v>
       </c>
       <c r="C134" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D134" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E134">
         <v>46742.5</v>
@@ -4824,7 +4836,7 @@
         <v>6.92119591378296</v>
       </c>
       <c r="I134" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -4835,10 +4847,10 @@
         <v>142</v>
       </c>
       <c r="C135" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D135" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E135">
         <v>344672.7272727273</v>
@@ -4853,7 +4865,7 @@
         <v>0.389485414358812</v>
       </c>
       <c r="I135" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="136" spans="1:9">
@@ -4864,10 +4876,10 @@
         <v>143</v>
       </c>
       <c r="C136" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D136" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E136">
         <v>61570</v>
@@ -4882,7 +4894,7 @@
         <v>1.847425694331655</v>
       </c>
       <c r="I136" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -4893,10 +4905,10 @@
         <v>144</v>
       </c>
       <c r="C137" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D137" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E137">
         <v>54420</v>
@@ -4911,7 +4923,7 @@
         <v>8.223171628077912</v>
       </c>
       <c r="I137" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -4922,10 +4934,10 @@
         <v>145</v>
       </c>
       <c r="C138" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D138" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E138">
         <v>67415</v>
@@ -4940,7 +4952,7 @@
         <v>1.898939405176889</v>
       </c>
       <c r="I138" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -4951,10 +4963,10 @@
         <v>146</v>
       </c>
       <c r="C139" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D139" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E139">
         <v>42281.82352941176</v>
@@ -4969,7 +4981,7 @@
         <v>1.034203266318026</v>
       </c>
       <c r="I139" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -4980,10 +4992,10 @@
         <v>147</v>
       </c>
       <c r="C140" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D140" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E140">
         <v>100666.6666666667</v>
@@ -4998,7 +5010,7 @@
         <v>1.986754966887417E-05</v>
       </c>
       <c r="I140" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -5009,10 +5021,10 @@
         <v>148</v>
       </c>
       <c r="C141" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D141" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E141">
         <v>43450</v>
@@ -5027,7 +5039,7 @@
         <v>4.532681242807825</v>
       </c>
       <c r="I141" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -5038,10 +5050,10 @@
         <v>149</v>
       </c>
       <c r="C142" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D142" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E142">
         <v>35630</v>
@@ -5056,7 +5068,7 @@
         <v>1.507690148751053</v>
       </c>
       <c r="I142" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -5067,10 +5079,10 @@
         <v>150</v>
       </c>
       <c r="C143" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D143" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E143">
         <v>60745</v>
@@ -5085,7 +5097,7 @@
         <v>0.8843361593546794</v>
       </c>
       <c r="I143" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -5096,10 +5108,10 @@
         <v>151</v>
       </c>
       <c r="C144" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D144" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E144">
         <v>27325.5</v>
@@ -5114,7 +5126,7 @@
         <v>1.084591315803919</v>
       </c>
       <c r="I144" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -5125,10 +5137,10 @@
         <v>152</v>
       </c>
       <c r="C145" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D145" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E145">
         <v>45105</v>
@@ -5143,7 +5155,7 @@
         <v>0.7998226360713889</v>
       </c>
       <c r="I145" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -5154,10 +5166,10 @@
         <v>153</v>
       </c>
       <c r="C146" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D146" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E146">
         <v>424480</v>
@@ -5172,7 +5184,7 @@
         <v>0.4647851488880513</v>
       </c>
       <c r="I146" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -5183,10 +5195,10 @@
         <v>154</v>
       </c>
       <c r="C147" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D147" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E147">
         <v>15610</v>
@@ -5201,7 +5213,7 @@
         <v>3.51947469570788</v>
       </c>
       <c r="I147" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -5212,10 +5224,10 @@
         <v>155</v>
       </c>
       <c r="C148" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D148" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E148">
         <v>18430</v>
@@ -5230,7 +5242,7 @@
         <v>3.958762886597938</v>
       </c>
       <c r="I148" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -5241,10 +5253,10 @@
         <v>156</v>
       </c>
       <c r="C149" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D149" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E149">
         <v>48439.80000000001</v>
@@ -5259,7 +5271,7 @@
         <v>4.052576600233691</v>
       </c>
       <c r="I149" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -5270,10 +5282,10 @@
         <v>157</v>
       </c>
       <c r="C150" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D150" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E150">
         <v>86620</v>
@@ -5288,7 +5300,7 @@
         <v>2.312918494574002</v>
       </c>
       <c r="I150" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -5299,10 +5311,10 @@
         <v>158</v>
       </c>
       <c r="C151" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D151" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E151">
         <v>36730</v>
@@ -5317,7 +5329,7 @@
         <v>1.161557310100735</v>
       </c>
       <c r="I151" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -5328,10 +5340,10 @@
         <v>159</v>
       </c>
       <c r="C152" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D152" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E152">
         <v>15280</v>
@@ -5346,7 +5358,7 @@
         <v>2.148821989528796</v>
       </c>
       <c r="I152" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -5357,10 +5369,10 @@
         <v>160</v>
       </c>
       <c r="C153" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D153" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E153">
         <v>63140</v>
@@ -5375,7 +5387,7 @@
         <v>1.49781438074121</v>
       </c>
       <c r="I153" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -5386,10 +5398,10 @@
         <v>161</v>
       </c>
       <c r="C154" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D154" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E154">
         <v>53706.66666666666</v>
@@ -5404,7 +5416,7 @@
         <v>3.88421052631579</v>
       </c>
       <c r="I154" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -5415,10 +5427,10 @@
         <v>162</v>
       </c>
       <c r="C155" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D155" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E155">
         <v>84169.8</v>
@@ -5433,7 +5445,7 @@
         <v>2.848907803036243</v>
       </c>
       <c r="I155" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -5444,10 +5456,10 @@
         <v>163</v>
       </c>
       <c r="C156" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D156" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E156">
         <v>219379.0363636363</v>
@@ -5462,7 +5474,7 @@
         <v>0.2116382712295291</v>
       </c>
       <c r="I156" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -5473,10 +5485,10 @@
         <v>164</v>
       </c>
       <c r="C157" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D157" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E157">
         <v>5000</v>
@@ -5491,7 +5503,7 @@
         <v>0.914</v>
       </c>
       <c r="I157" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -5502,10 +5514,10 @@
         <v>165</v>
       </c>
       <c r="C158" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D158" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E158">
         <v>68881.36363636363</v>
@@ -5520,7 +5532,7 @@
         <v>6.753553870620765</v>
       </c>
       <c r="I158" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="159" spans="1:9">
@@ -5531,10 +5543,10 @@
         <v>166</v>
       </c>
       <c r="C159" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D159" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E159">
         <v>352072.5</v>
@@ -5549,7 +5561,7 @@
         <v>0</v>
       </c>
       <c r="I159" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -5560,10 +5572,10 @@
         <v>167</v>
       </c>
       <c r="C160" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D160" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E160">
         <v>112588.4615384615</v>
@@ -5578,7 +5590,7 @@
         <v>0.0004352133365217095</v>
       </c>
       <c r="I160" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -5589,10 +5601,10 @@
         <v>168</v>
       </c>
       <c r="C161" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D161" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E161">
         <v>24826.15384615385</v>
@@ -5607,7 +5619,7 @@
         <v>7.837984135836896</v>
       </c>
       <c r="I161" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -5618,10 +5630,10 @@
         <v>169</v>
       </c>
       <c r="C162" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D162" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E162">
         <v>113740</v>
@@ -5636,7 +5648,7 @@
         <v>2.21310005275189</v>
       </c>
       <c r="I162" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -5647,10 +5659,10 @@
         <v>170</v>
       </c>
       <c r="C163" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D163" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E163">
         <v>56545</v>
@@ -5665,7 +5677,123 @@
         <v>5.138827482536033</v>
       </c>
       <c r="I163" t="s">
-        <v>187</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9">
+      <c r="A164">
+        <v>237674841555</v>
+      </c>
+      <c r="B164" t="s">
+        <v>171</v>
+      </c>
+      <c r="C164" t="s">
+        <v>181</v>
+      </c>
+      <c r="D164" t="s">
+        <v>190</v>
+      </c>
+      <c r="E164">
+        <v>150379.6</v>
+      </c>
+      <c r="F164">
+        <v>790555</v>
+      </c>
+      <c r="G164">
+        <v>640175.4</v>
+      </c>
+      <c r="H164">
+        <v>5.257062793091616</v>
+      </c>
+      <c r="I164" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
+      <c r="A165">
+        <v>237674899678</v>
+      </c>
+      <c r="B165" t="s">
+        <v>172</v>
+      </c>
+      <c r="C165" t="s">
+        <v>181</v>
+      </c>
+      <c r="D165" t="s">
+        <v>190</v>
+      </c>
+      <c r="E165">
+        <v>159035.175</v>
+      </c>
+      <c r="F165">
+        <v>507599</v>
+      </c>
+      <c r="G165">
+        <v>348563.825</v>
+      </c>
+      <c r="H165">
+        <v>3.191740443584258</v>
+      </c>
+      <c r="I165" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9">
+      <c r="A166">
+        <v>237676439452</v>
+      </c>
+      <c r="B166" t="s">
+        <v>173</v>
+      </c>
+      <c r="C166" t="s">
+        <v>181</v>
+      </c>
+      <c r="D166" t="s">
+        <v>190</v>
+      </c>
+      <c r="E166">
+        <v>87377.35000000001</v>
+      </c>
+      <c r="F166">
+        <v>9597</v>
+      </c>
+      <c r="G166">
+        <v>-77780.35000000001</v>
+      </c>
+      <c r="H166">
+        <v>0.1098339558249363</v>
+      </c>
+      <c r="I166" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9">
+      <c r="A167">
+        <v>237676695935</v>
+      </c>
+      <c r="B167" t="s">
+        <v>174</v>
+      </c>
+      <c r="C167" t="s">
+        <v>181</v>
+      </c>
+      <c r="D167" t="s">
+        <v>190</v>
+      </c>
+      <c r="E167">
+        <v>88445</v>
+      </c>
+      <c r="F167">
+        <v>312534</v>
+      </c>
+      <c r="G167">
+        <v>224089</v>
+      </c>
+      <c r="H167">
+        <v>3.53365368307988</v>
+      </c>
+      <c r="I167" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>